<commit_message>
[Jihwan] add Player Animation, add Voxel FX, add Player Attack
</commit_message>
<xml_diff>
--- a/DeepDarkDungeon/Assets/01_DeepDarkDungeon/Resources/Datas/ItemDB.xlsx
+++ b/DeepDarkDungeon/Assets/01_DeepDarkDungeon/Resources/Datas/ItemDB.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jahni\Unity\0803_DeepDarkDungeon\DeepDarkDungeon_Main\DeepDarkDungeon\Assets\01_DeepDarkDungeon\Resources\Datas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jihwan\Works\Unity\0803_DeepDarkDungeon\DeeoDarkDungeon\DeepDarkDungeon\Assets\01_DeepDarkDungeon\Resources\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9BBD3DB-27A3-4424-BC7E-D446199E7EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8040"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>value</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -86,26 +87,22 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Melee</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Melee</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DarkSword</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Hammer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TwohandSword</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -428,20 +425,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="F4" sqref="F3:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="12.125" customWidth="1"/>
+    <col min="3" max="3" width="12.08203125" customWidth="1"/>
+    <col min="6" max="6" width="18.9140625" customWidth="1"/>
     <col min="8" max="8" width="14.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -467,12 +465,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
@@ -486,7 +484,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>2</v>
       </c>
@@ -503,7 +501,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>3</v>
       </c>
@@ -511,7 +509,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -520,7 +518,7 @@
         <v>300</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G5">
         <v>10</v>
@@ -529,7 +527,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>4</v>
       </c>
@@ -546,7 +544,7 @@
         <v>500</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G6">
         <v>20</v>
@@ -555,7 +553,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>5</v>
       </c>
@@ -572,7 +570,7 @@
         <v>800</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="G7">
         <v>30</v>
@@ -581,7 +579,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>6</v>
       </c>
@@ -589,7 +587,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -598,7 +596,7 @@
         <v>1000</v>
       </c>
       <c r="F8" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="G8">
         <v>50</v>

</xml_diff>

<commit_message>
[Jihwan] Fix Camera Cinemachine, Fix Player
</commit_message>
<xml_diff>
--- a/DeepDarkDungeon/Assets/01_DeepDarkDungeon/Resources/Datas/ItemDB.xlsx
+++ b/DeepDarkDungeon/Assets/01_DeepDarkDungeon/Resources/Datas/ItemDB.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jihwan\Works\Unity\0803_DeepDarkDungeon\DeeoDarkDungeon\DeepDarkDungeon\Assets\01_DeepDarkDungeon\Resources\Datas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jahni\Unity\0803_DeepDarkDungeon\DeepDarkDungeon_Main\DeepDarkDungeon\Assets\01_DeepDarkDungeon\Resources\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9BBD3DB-27A3-4424-BC7E-D446199E7EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="765" yWindow="765" windowWidth="28800" windowHeight="15465"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -102,7 +101,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -425,21 +424,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F3:F4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="12.08203125" customWidth="1"/>
-    <col min="6" max="6" width="18.9140625" customWidth="1"/>
+    <col min="3" max="3" width="12.125" customWidth="1"/>
+    <col min="6" max="6" width="18.875" customWidth="1"/>
     <col min="8" max="8" width="14.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -465,12 +464,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -484,7 +483,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -501,7 +500,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -527,7 +526,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -553,7 +552,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -579,7 +578,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
[Jihwan] Add Title Img, Fix Player Attack, Fix Spawn Room, Add Trap Room, Add Boss UI, Fix Boss Room, Fix Exit Room, Fix Weapon
</commit_message>
<xml_diff>
--- a/DeepDarkDungeon/Assets/01_DeepDarkDungeon/Resources/Datas/ItemDB.xlsx
+++ b/DeepDarkDungeon/Assets/01_DeepDarkDungeon/Resources/Datas/ItemDB.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jahni\Unity\0803_DeepDarkDungeon\DeepDarkDungeon_Main\DeepDarkDungeon\Assets\01_DeepDarkDungeon\Resources\Datas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jihwan\Works\Unity\0803_DeepDarkDungeon\DeeoDarkDungeon\DeepDarkDungeon\Assets\01_DeepDarkDungeon\Resources\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{196CE359-4B32-42FE-A4B9-F053A6FA4E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="765" yWindow="765" windowWidth="28800" windowHeight="15465"/>
+    <workbookView xWindow="3040" yWindow="3040" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -101,7 +102,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -424,21 +425,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="12.125" customWidth="1"/>
-    <col min="6" max="6" width="18.875" customWidth="1"/>
+    <col min="3" max="3" width="12.08203125" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" customWidth="1"/>
     <col min="8" max="8" width="14.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -464,12 +465,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
@@ -480,10 +481,10 @@
         <v>10</v>
       </c>
       <c r="D3">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>2</v>
       </c>
@@ -500,7 +501,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>3</v>
       </c>
@@ -520,13 +521,13 @@
         <v>17</v>
       </c>
       <c r="G5">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H5">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>4</v>
       </c>
@@ -546,13 +547,13 @@
         <v>5</v>
       </c>
       <c r="G6">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="H6">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>5</v>
       </c>
@@ -572,13 +573,13 @@
         <v>6</v>
       </c>
       <c r="G7">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H7">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
[Jihwan] Add Sound Option UI, Add Items, Fix Monster KnockBack, Add Monster Death Effect
</commit_message>
<xml_diff>
--- a/DeepDarkDungeon/Assets/01_DeepDarkDungeon/Resources/Datas/ItemDB.xlsx
+++ b/DeepDarkDungeon/Assets/01_DeepDarkDungeon/Resources/Datas/ItemDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jihwan\Works\Unity\0803_DeepDarkDungeon\DeeoDarkDungeon\DeepDarkDungeon\Assets\01_DeepDarkDungeon\Resources\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{196CE359-4B32-42FE-A4B9-F053A6FA4E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364166BD-F2F2-4879-9E4F-0953E681263A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3040" yWindow="3040" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>value</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -96,6 +96,21 @@
   </si>
   <si>
     <t>TwohandSword</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Speed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Power</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shield</t>
+  </si>
+  <si>
+    <t>Shield</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -426,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -506,25 +521,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
         <v>300</v>
-      </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5">
-        <v>20</v>
-      </c>
-      <c r="H5">
-        <v>1.3</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
@@ -532,25 +538,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>500</v>
-      </c>
-      <c r="F6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6">
-        <v>10</v>
-      </c>
-      <c r="H6">
-        <v>0.8</v>
+        <v>400</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
@@ -558,16 +555,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>800</v>
+        <v>500</v>
       </c>
       <c r="F7" t="s">
         <v>6</v>
@@ -583,26 +580,129 @@
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
         <v>2</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>300</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12">
+        <v>20</v>
+      </c>
+      <c r="H12">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>500</v>
+      </c>
+      <c r="F13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13">
+        <v>10</v>
+      </c>
+      <c r="H13">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>800</v>
+      </c>
+      <c r="F14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14">
+        <v>50</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
         <v>15</v>
       </c>
-      <c r="D8">
+      <c r="D15">
         <v>3</v>
       </c>
-      <c r="E8">
+      <c r="E15">
         <v>1000</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F15" t="s">
         <v>5</v>
       </c>
-      <c r="G8">
+      <c r="G15">
         <v>50</v>
       </c>
-      <c r="H8">
+      <c r="H15">
         <v>0.4</v>
+      </c>
+    </row>
+    <row r="17" spans="11:11" x14ac:dyDescent="0.45">
+      <c r="K17">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Jihwan] Fix Save System, Add PostProcessing, Add Camera
</commit_message>
<xml_diff>
--- a/DeepDarkDungeon/Assets/01_DeepDarkDungeon/Resources/Datas/ItemDB.xlsx
+++ b/DeepDarkDungeon/Assets/01_DeepDarkDungeon/Resources/Datas/ItemDB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jihwan\Works\Unity\0803_DeepDarkDungeon\DeeoDarkDungeon\DeepDarkDungeon\Assets\01_DeepDarkDungeon\Resources\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364166BD-F2F2-4879-9E4F-0953E681263A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70453FF-626E-44A0-AF0A-99C039991352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3040" yWindow="3040" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21320" yWindow="2380" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
   <si>
     <t>value</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -441,16 +441,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="12.08203125" customWidth="1"/>
-    <col min="6" max="6" width="18.83203125" customWidth="1"/>
+    <col min="6" max="6" width="13.25" customWidth="1"/>
     <col min="8" max="8" width="14.25" customWidth="1"/>
   </cols>
   <sheetData>
@@ -700,8 +700,91 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="17" spans="11:11" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>300</v>
+      </c>
+      <c r="F16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>300</v>
+      </c>
+      <c r="F17" t="s">
+        <v>5</v>
+      </c>
       <c r="K17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>6</v>
+      </c>
+      <c r="E18">
+        <v>300</v>
+      </c>
+      <c r="F18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>7</v>
+      </c>
+      <c r="E19">
+        <v>300</v>
+      </c>
+      <c r="F19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>8</v>
+      </c>
+      <c r="E20">
+        <v>300</v>
+      </c>
+      <c r="F20" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Jihwan] Fix ItemSlot, Add Weapon, Add Cinemachine, Fix UI
</commit_message>
<xml_diff>
--- a/DeepDarkDungeon/Assets/01_DeepDarkDungeon/Resources/Datas/ItemDB.xlsx
+++ b/DeepDarkDungeon/Assets/01_DeepDarkDungeon/Resources/Datas/ItemDB.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jihwan\Works\Unity\0803_DeepDarkDungeon\DeeoDarkDungeon\DeepDarkDungeon\Assets\01_DeepDarkDungeon\Resources\Datas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jahni\Unity\0803_DeepDarkDungeon\DeepDarkDungeon_Main\DeepDarkDungeon\Assets\01_DeepDarkDungeon\Resources\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70453FF-626E-44A0-AF0A-99C039991352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21320" yWindow="2380" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21315" yWindow="2385" windowWidth="28800" windowHeight="15465"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
   <si>
     <t>value</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -87,37 +86,49 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Hammer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TwohandSword</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Speed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Power</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shield</t>
+  </si>
+  <si>
+    <t>Shield</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mace</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mace</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>DarkSword</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Hammer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TwohandSword</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Speed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Power</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shield</t>
-  </si>
-  <si>
-    <t>Shield</t>
+    <t>ForestMourn</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -440,21 +451,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15:F20"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="12.08203125" customWidth="1"/>
+    <col min="3" max="3" width="12.125" customWidth="1"/>
     <col min="6" max="6" width="13.25" customWidth="1"/>
     <col min="8" max="8" width="14.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -480,12 +491,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -499,7 +510,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -516,15 +527,15 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -533,15 +544,15 @@
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
         <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -550,15 +561,15 @@
         <v>400</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -576,27 +587,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -604,7 +615,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -613,7 +624,7 @@
         <v>300</v>
       </c>
       <c r="F12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G12">
         <v>20</v>
@@ -622,7 +633,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -648,7 +659,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -668,13 +679,13 @@
         <v>6</v>
       </c>
       <c r="G14">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="H14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -682,7 +693,7 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D15">
         <v>3</v>
@@ -700,30 +711,42 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>2</v>
       </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
       <c r="D16">
         <v>4</v>
       </c>
       <c r="E16">
-        <v>300</v>
+        <v>2000</v>
       </c>
       <c r="F16" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+        <v>16</v>
+      </c>
+      <c r="G16">
+        <v>100</v>
+      </c>
+      <c r="H16">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>2</v>
       </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
       <c r="D17">
         <v>5</v>
       </c>
@@ -731,61 +754,40 @@
         <v>300</v>
       </c>
       <c r="F17" t="s">
-        <v>5</v>
+        <v>21</v>
+      </c>
+      <c r="G17">
+        <v>15</v>
+      </c>
+      <c r="H17">
+        <v>0.4</v>
       </c>
       <c r="K17">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" t="s">
         <v>2</v>
       </c>
-      <c r="D18">
-        <v>6</v>
-      </c>
-      <c r="E18">
-        <v>300</v>
-      </c>
-      <c r="F18" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>2</v>
       </c>
-      <c r="D19">
-        <v>7</v>
-      </c>
-      <c r="E19">
-        <v>300</v>
-      </c>
-      <c r="F19" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>2</v>
-      </c>
-      <c r="D20">
-        <v>8</v>
-      </c>
-      <c r="E20">
-        <v>300</v>
-      </c>
-      <c r="F20" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Jihwan] Add Item UI, Add Sign, Add Spike, Fix Weapon, Fix Mage Materials
</commit_message>
<xml_diff>
--- a/DeepDarkDungeon/Assets/01_DeepDarkDungeon/Resources/Datas/ItemDB.xlsx
+++ b/DeepDarkDungeon/Assets/01_DeepDarkDungeon/Resources/Datas/ItemDB.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jahni\Unity\0803_DeepDarkDungeon\DeepDarkDungeon_Main\DeepDarkDungeon\Assets\01_DeepDarkDungeon\Resources\Datas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Jihwan\Works\Unity\0803_DeepDarkDungeon\DeeoDarkDungeon\DeepDarkDungeon\Assets\01_DeepDarkDungeon\Resources\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{247C65B2-AF33-4A94-8339-CFF5357E0FBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21315" yWindow="2385" windowWidth="28800" windowHeight="15465"/>
+    <workbookView xWindow="3800" yWindow="3800" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
   <si>
     <t>value</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -38,10 +39,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>type</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -74,10 +71,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Heart</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>rate</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -86,10 +79,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Hammer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>TwohandSword</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -105,30 +94,58 @@
     <t>Shield</t>
   </si>
   <si>
-    <t>Shield</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Mace</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Mace</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DarkSword</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ForestMourn</t>
+    <t>itemName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하트 | HP 50+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>실드 |  방어력+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이동속도 +</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파워 +</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뿅망치</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>낡은 검</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>체인-쏘우</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다크 소드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서리한</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>철퇴</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -451,29 +468,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="12.125" customWidth="1"/>
+    <col min="3" max="3" width="12.08203125" customWidth="1"/>
     <col min="6" max="6" width="13.25" customWidth="1"/>
     <col min="8" max="8" width="14.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -482,43 +499,43 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
       </c>
       <c r="D3">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D4">
         <v>50</v>
@@ -527,15 +544,15 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -544,12 +561,12 @@
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
@@ -561,15 +578,15 @@
         <v>400</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -578,7 +595,7 @@
         <v>500</v>
       </c>
       <c r="F7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G7">
         <v>50</v>
@@ -587,27 +604,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>10</v>
       </c>
@@ -615,7 +632,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -624,7 +641,7 @@
         <v>300</v>
       </c>
       <c r="F12" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G12">
         <v>20</v>
@@ -633,7 +650,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>11</v>
       </c>
@@ -641,7 +658,7 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -650,7 +667,7 @@
         <v>500</v>
       </c>
       <c r="F13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G13">
         <v>10</v>
@@ -659,7 +676,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>12</v>
       </c>
@@ -667,7 +684,7 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D14">
         <v>2</v>
@@ -676,7 +693,7 @@
         <v>800</v>
       </c>
       <c r="F14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G14">
         <v>25</v>
@@ -685,7 +702,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>13</v>
       </c>
@@ -693,7 +710,7 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D15">
         <v>3</v>
@@ -702,7 +719,7 @@
         <v>1000</v>
       </c>
       <c r="F15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G15">
         <v>50</v>
@@ -711,7 +728,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>14</v>
       </c>
@@ -719,7 +736,7 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D16">
         <v>4</v>
@@ -728,7 +745,7 @@
         <v>2000</v>
       </c>
       <c r="F16" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G16">
         <v>100</v>
@@ -737,7 +754,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>15</v>
       </c>
@@ -745,16 +762,16 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D17">
         <v>5</v>
       </c>
       <c r="E17">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="F17" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G17">
         <v>15</v>
@@ -762,11 +779,8 @@
       <c r="H17">
         <v>0.4</v>
       </c>
-      <c r="K17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>16</v>
       </c>
@@ -774,7 +788,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>17</v>
       </c>
@@ -782,7 +796,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>18</v>
       </c>

</xml_diff>